<commit_message>
Update app and add docker
</commit_message>
<xml_diff>
--- a/data/NetworkFlowProblem-Data.xlsx
+++ b/data/NetworkFlowProblem-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\bryce\code\corteva\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61860C95-EA62-4DD4-BFC7-6DCB6015F411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C5C06A-4F00-4360-B0C5-61941587A79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{E3F19191-E47E-4C86-B9D1-D2E4449E062A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E3F19191-E47E-4C86-B9D1-D2E4449E062A}"/>
   </bookViews>
   <sheets>
     <sheet name="Input1" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,6 @@
     <sheet name="Input3" sheetId="5" r:id="rId5"/>
     <sheet name="Input4" sheetId="6" r:id="rId6"/>
     <sheet name="Input5" sheetId="8" r:id="rId7"/>
-    <sheet name="Input6" sheetId="10" r:id="rId8"/>
-    <sheet name="Input6bak" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Input1!$E$1:$E$49</definedName>
@@ -47,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="42">
   <si>
     <t>send_from_cnt</t>
   </si>
@@ -333,44 +331,6 @@
     <tableColumn id="5" xr3:uid="{E6B06DF7-B9FF-40B9-A602-19E1BD0A63F1}" name="for_process"/>
     <tableColumn id="6" xr3:uid="{A8AE3640-4998-4A70-A02A-55BCBE94D924}" name="Week"/>
     <tableColumn id="7" xr3:uid="{EA5A27F4-CB39-48D9-862E-71CB5609DF51}" name="Amount"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AC75B4BC-36AC-4735-9735-5C13E50A323D}" name="Table134" displayName="Table134" ref="A1:G10" totalsRowShown="0">
-  <autoFilter ref="A1:G10" xr:uid="{748CE9DF-C4A7-4CA7-955A-C31BEE0FDE96}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G7">
-    <sortCondition ref="E1:E7"/>
-  </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3394FBA0-E4EA-4F7D-954E-488E2076B49E}" name="product"/>
-    <tableColumn id="2" xr3:uid="{F4446891-38AD-4D17-B206-4C8FEDD1E235}" name="treatment"/>
-    <tableColumn id="3" xr3:uid="{E3B09C50-6CE6-44B9-A97B-20BD1E97BE2A}" name="send_from_cnt"/>
-    <tableColumn id="4" xr3:uid="{BA628021-E7EA-40F7-9418-01666984D92D}" name="to_processing_cnt"/>
-    <tableColumn id="5" xr3:uid="{0CF7E800-DA82-47D3-9790-DFB45ED06CF6}" name="for_process"/>
-    <tableColumn id="6" xr3:uid="{635C941A-FE0C-4419-A868-2725E5404599}" name="Week"/>
-    <tableColumn id="7" xr3:uid="{03E5E7E5-3989-4BA9-9E66-00EA1D8E39C4}" name="Amount"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{748CE9DF-C4A7-4CA7-955A-C31BEE0FDE96}" name="Table13" displayName="Table13" ref="A1:G10" totalsRowShown="0">
-  <autoFilter ref="A1:G10" xr:uid="{748CE9DF-C4A7-4CA7-955A-C31BEE0FDE96}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G10">
-    <sortCondition ref="E1:E10"/>
-  </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{8933C7A2-2B55-4EC5-81A2-1A455CA568B4}" name="product"/>
-    <tableColumn id="2" xr3:uid="{472C68B3-DE6F-4CB1-B89E-EB3DE17607DF}" name="treatment"/>
-    <tableColumn id="3" xr3:uid="{6AE7AED1-047D-4D6E-9082-6104E4E69FA3}" name="send_from_cnt"/>
-    <tableColumn id="4" xr3:uid="{B759889B-6CEF-48A2-8B39-DFAA791577BB}" name="to_processing_cnt"/>
-    <tableColumn id="5" xr3:uid="{FE4C60C6-A521-449F-88F6-8348008EB4FF}" name="for_process"/>
-    <tableColumn id="6" xr3:uid="{1EC57566-A1D7-4D8A-9B64-0C26B55A1829}" name="Week"/>
-    <tableColumn id="7" xr3:uid="{4E45017E-E56C-428C-BEA4-56B90FF24D4F}" name="Amount"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -675,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA089E0-D283-4783-9B52-67650476778B}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,8 +1776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01C61485-64A7-4B7F-B8D3-D34E95743FBD}">
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2824,6 +2784,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3020,7 +2983,7 @@
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3233,8 +3196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31E6CE7-DC96-4823-A695-12E363B62A0D}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3744,10 +3707,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B29D59-2288-4D87-BA2B-9AC3D0CFF30D}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3760,638 +3723,6 @@
     <col min="7" max="7" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1064.81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1462.82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>124.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>6675.88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>47.19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7">
-        <v>13</v>
-      </c>
-      <c r="G7">
-        <v>124.3</v>
-      </c>
-      <c r="I7">
-        <f>SUM(G7:G10)</f>
-        <v>9374.9999999999927</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8">
-        <v>18</v>
-      </c>
-      <c r="G8">
-        <v>6723.07</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9">
-        <v>23</v>
-      </c>
-      <c r="G9">
-        <v>1854.53000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10">
-        <v>24</v>
-      </c>
-      <c r="G10">
-        <v>673.09999999998195</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11">
-        <v>8</v>
-      </c>
-      <c r="G11">
-        <v>124.3</v>
-      </c>
-      <c r="I11">
-        <f>SUM(G11:G15)</f>
-        <v>9374.9999999999927</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12">
-        <v>11</v>
-      </c>
-      <c r="G12">
-        <v>1623.48000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13">
-        <v>12</v>
-      </c>
-      <c r="G13">
-        <v>231.049999999991</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14">
-        <v>14</v>
-      </c>
-      <c r="G14">
-        <v>673.09999999998195</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15">
-        <v>14</v>
-      </c>
-      <c r="G15">
-        <v>6723.07</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>1064.81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1462.82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>124.3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>6675.88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>47.19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21">
-        <v>4</v>
-      </c>
-      <c r="G21">
-        <v>124.3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22">
-        <v>5</v>
-      </c>
-      <c r="G22">
-        <v>911.480000000019</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23">
-        <v>6</v>
-      </c>
-      <c r="G23">
-        <v>231.049999999991</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24">
-        <v>7</v>
-      </c>
-      <c r="G24">
-        <v>712.00000000000603</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25">
-        <v>9</v>
-      </c>
-      <c r="G25">
-        <v>320.28999999998899</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26">
-        <v>10</v>
-      </c>
-      <c r="G26">
-        <v>352.80999999999301</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27">
-        <v>10</v>
-      </c>
-      <c r="G27">
-        <v>6723.07</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC7438B-3BC8-4F4E-858A-94C692151807}">
-  <dimension ref="A1:G10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
@@ -4423,19 +3754,19 @@
         <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F2">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>124.3</v>
+        <v>1064.81</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4446,19 +3777,19 @@
         <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>124.3</v>
+        <v>1462.82</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4469,19 +3800,19 @@
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F4">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>6723.07</v>
+        <v>124.3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -4492,19 +3823,19 @@
         <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F5">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>6723.07</v>
+        <v>6675.88</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -4515,19 +3846,19 @@
         <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F6">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>673.09999999998195</v>
+        <v>47.19</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -4538,19 +3869,19 @@
         <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
         <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F7">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7">
-        <v>673.09999999998195</v>
+        <v>124.3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -4561,7 +3892,7 @@
         <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
         <v>40</v>
@@ -4570,10 +3901,10 @@
         <v>17</v>
       </c>
       <c r="F8">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G8">
-        <v>1854.53000000001</v>
+        <v>6723.07</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -4584,19 +3915,19 @@
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
         <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F9">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="G9">
-        <v>1623.48000000002</v>
+        <v>1854.53000000001</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4607,266 +3938,394 @@
         <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
         <v>40</v>
       </c>
       <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10">
+        <v>24</v>
+      </c>
+      <c r="G10">
+        <v>673.09999999998195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
         <v>16</v>
       </c>
-      <c r="F10">
+      <c r="F11">
+        <v>8</v>
+      </c>
+      <c r="G11">
+        <v>124.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <v>11</v>
+      </c>
+      <c r="G12">
+        <v>1623.48000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13">
         <v>12</v>
       </c>
-      <c r="G10">
+      <c r="G13">
         <v>231.049999999991</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E4566E-D787-4ECE-AE8C-89A52B456925}">
-  <dimension ref="A1:G10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="A7:G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14">
+        <v>14</v>
+      </c>
+      <c r="G14">
+        <v>673.09999999998195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>6723.07</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1064.81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1462.82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>124.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>6675.88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>47.19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="G21">
+        <v>124.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C22" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2">
-        <v>13</v>
-      </c>
-      <c r="G2">
-        <v>124.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <v>911.480000000019</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
         <v>41</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C23" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3">
+      <c r="D23" t="s">
         <v>18</v>
       </c>
-      <c r="G3">
-        <v>6723.07</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23">
+        <v>6</v>
+      </c>
+      <c r="G23">
+        <v>231.049999999991</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
         <v>41</v>
       </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4">
-        <v>23</v>
-      </c>
-      <c r="G4">
-        <v>1854.53000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24">
+        <v>7</v>
+      </c>
+      <c r="G24">
+        <v>712.00000000000603</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
         <v>41</v>
       </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5">
-        <v>24</v>
-      </c>
-      <c r="G5">
-        <v>673.09999999998195</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25">
+        <v>9</v>
+      </c>
+      <c r="G25">
+        <v>320.28999999998899</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
         <v>41</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6">
-        <v>8</v>
-      </c>
-      <c r="G6">
-        <v>124.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26">
+        <v>10</v>
+      </c>
+      <c r="G26">
+        <v>352.80999999999301</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
         <v>41</v>
       </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7">
-        <v>11</v>
-      </c>
-      <c r="G7">
-        <v>1623.48000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8">
-        <v>12</v>
-      </c>
-      <c r="G8">
-        <v>231.049999999991</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9">
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s">
         <v>14</v>
       </c>
-      <c r="G9">
-        <v>673.09999999998195</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10">
-        <v>14</v>
-      </c>
-      <c r="G10">
+      <c r="F27">
+        <v>10</v>
+      </c>
+      <c r="G27">
         <v>6723.07</v>
       </c>
     </row>

</xml_diff>